<commit_message>
Formatted/linted. Format blank rows as text
</commit_message>
<xml_diff>
--- a/template-generator/USDM_Test_Data_Template.xlsx
+++ b/template-generator/USDM_Test_Data_Template.xlsx
@@ -1095,6 +1095,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="@"/>
+  </numFmts>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -1166,7 +1169,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>

</xml_diff>